<commit_message>
Added test case CMC Autopay 2.7 version and created keyword class for mutilbill search and cart content page
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D1DDD338-6C8D-40DA-96CE-789CE3818063}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{88710B78-9931-456F-B791-5CCD45D30994}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="8" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView activeTab="14" firstSheet="11" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowNoCFPC_27" r:id="rId1" sheetId="1"/>
@@ -25,6 +25,9 @@
     <sheet name="CCDeferredPS_27" r:id="rId10" sheetId="10"/>
     <sheet name="CCDeferredPC_27" r:id="rId11" sheetId="11"/>
     <sheet name="CCDeferredCorp_27" r:id="rId12" sheetId="12"/>
+    <sheet name="CMCAutopayPC_27" r:id="rId13" sheetId="13"/>
+    <sheet name="CMCAutopayCorp_27" r:id="rId14" sheetId="14"/>
+    <sheet name="CMCAutopayPS_27" r:id="rId15" sheetId="15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="48">
   <si>
     <t>Result</t>
   </si>
@@ -155,13 +158,31 @@
     <t>Fri Jan 24 15:44:49 IST 2025</t>
   </si>
   <si>
+    <t>Fri Jan 24 15:53:59 IST 2025</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Wed Jan 29 17:54:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Dec 17 17:33:30 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 17 15:47:30 IST 2024</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Fri Jan 24 15:53:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Jan 24 15:53:59 IST 2025</t>
+    <t>Tue Feb 04 19:13:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Feb 04 19:16:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 05 17:20:04 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -812,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33510FF-D609-4CBB-88F3-62D4AD35558D}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -867,7 +888,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -902,6 +923,297 @@
       </c>
       <c r="N2" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2F5EF4-293E-4FBA-854F-4D8FBFA201D5}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C34E9A6-18FA-47DA-8CAD-7C400147C1DF}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1B9718-D45F-4DCA-9C3D-3DEA47AFA8B0}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1508,7 +1820,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N2"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Multibill Verification test case
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="52">
   <si>
     <t>Result</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>Wed Feb 05 17:20:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 12 15:14:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 12 15:15:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 12 15:18:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 12 15:21:32 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -986,10 +998,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1083,10 +1095,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1180,10 +1192,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Added test cases of Multibill,created Multibill regression suite,Updated CCdeferred payments as CMCDeffered in 2.7 version
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="95">
   <si>
     <t>Result</t>
   </si>
@@ -195,6 +195,135 @@
   </si>
   <si>
     <t>Wed Feb 12 15:21:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:02:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:04:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:05:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:10:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:12:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:14:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:21:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:22:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:23:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:26:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:28:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:29:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:31:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:32:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 26 16:33:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Feb 27 20:46:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Feb 27 20:50:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Feb 27 20:57:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Feb 27 21:01:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 14:40:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 14:44:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 14:47:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 06 15:32:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 06 15:34:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 06 16:50:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 06 16:51:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 06 16:56:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 06 17:11:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 14:48:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 14:50:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 14:51:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 14:56:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 14:58:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:00:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:04:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:06:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:07:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:10:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:11:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:12:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:15:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:15:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 15:17:15 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -587,10 +716,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -695,7 +824,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -799,7 +928,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -900,7 +1029,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1001,7 +1130,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1098,7 +1227,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1195,7 +1324,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1289,10 +1418,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1391,7 +1520,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1490,7 +1619,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1589,7 +1718,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1688,7 +1817,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1787,7 +1916,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1886,7 +2015,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1985,7 +2114,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Added ABP Object repository,Keyword Classes and ABP test cases
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsACH_27.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="178">
   <si>
     <t>Result</t>
   </si>
@@ -324,6 +324,255 @@
   </si>
   <si>
     <t>Wed Mar 26 15:17:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:00:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:02:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:03:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:08:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:10:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:12:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:16:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:18:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:19:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:22:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:23:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:24:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:27:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:27:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Apr 07 21:29:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:29:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:31:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:33:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:37:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:39:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:41:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:43:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:44:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:45:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:47:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:48:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:49:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:50:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:51:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 02 21:51:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 12:39:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 12:55:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 12:55:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 12:55:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 13:10:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 13:17:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 04 13:23:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:38:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:41:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:43:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:47:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:49:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:51:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:54:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:55:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:56:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:58:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:59:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 11:59:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 12:01:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 12:02:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 12:02:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 19:37:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 19:40:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 05 21:59:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jun 06 11:03:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:17:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:18:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:18:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:20:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:36:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:37:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:45:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:54:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 11:55:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 12:01:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:25:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:25:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:48:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:49:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:56:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:57:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 14:58:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 15:39:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 15:44:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 15:44:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 20:28:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 10 20:28:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 17 11:11:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 17 11:13:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 17 11:14:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 17 11:30:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jun 17 11:38:24 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -719,7 +968,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -821,10 +1070,10 @@
     </row>
     <row ht="29" r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -925,10 +1174,10 @@
     </row>
     <row ht="29" r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1029,7 +1278,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1130,7 +1379,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1227,7 +1476,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1324,7 +1573,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1421,7 +1670,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1520,7 +1769,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1619,7 +1868,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1718,7 +1967,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1817,7 +2066,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1916,7 +2165,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2015,7 +2264,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2114,7 +2363,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">

</xml_diff>